<commit_message>
GiovanniLap: Viernes 29 de Enero de 2016
</commit_message>
<xml_diff>
--- a/docs/ControlPersistencia.xlsx
+++ b/docs/ControlPersistencia.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="90" windowWidth="14055" windowHeight="5130"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
   <si>
     <t>Nombre</t>
   </si>
@@ -55,13 +55,34 @@
   </si>
   <si>
     <t>Controller</t>
+  </si>
+  <si>
+    <t>Domicilio</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Fiscales</t>
+  </si>
+  <si>
+    <t>Municipio</t>
+  </si>
+  <si>
+    <t>Telefono</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,12 +91,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -90,14 +117,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -176,6 +210,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -210,6 +245,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,19 +421,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -420,7 +456,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -440,7 +476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -460,7 +496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -483,7 +519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -500,6 +536,131 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
         <v>7</v>
       </c>
     </row>
@@ -509,24 +670,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
GiovanniPC: Lunes 1 de Febrero de 2016
</commit_message>
<xml_diff>
--- a/docs/ControlPersistencia.xlsx
+++ b/docs/ControlPersistencia.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="90" windowWidth="14055" windowHeight="5130"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Controllers" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Persistencia" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
   <si>
     <t>Nombre</t>
   </si>
@@ -76,16 +76,116 @@
   </si>
   <si>
     <t>Telefono</t>
+  </si>
+  <si>
+    <t>Vista</t>
+  </si>
+  <si>
+    <t>Encuesta</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>alta</t>
+  </si>
+  <si>
+    <t>edita</t>
+  </si>
+  <si>
+    <t>baja</t>
+  </si>
+  <si>
+    <t>secciones</t>
+  </si>
+  <si>
+    <t>index.phtml</t>
+  </si>
+  <si>
+    <t>admin.phtml</t>
+  </si>
+  <si>
+    <t>alta.phtml</t>
+  </si>
+  <si>
+    <t>edita.phtml</t>
+  </si>
+  <si>
+    <t>baja.phtml</t>
+  </si>
+  <si>
+    <t>secciones.phtml</t>
+  </si>
+  <si>
+    <t>Seccion</t>
+  </si>
+  <si>
+    <t>Params</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>idEncuesta</t>
+  </si>
+  <si>
+    <t>idSeccion</t>
+  </si>
+  <si>
+    <t>Objetivo</t>
+  </si>
+  <si>
+    <t>Mostrar encuestas activas en el modulo, navegación directa a: encuesta/index/alta</t>
+  </si>
+  <si>
+    <t>Edita encuesta y redirecciona a encuesta/index/admin/+param</t>
+  </si>
+  <si>
+    <t>Elimina encuesta y redirecciona a encuesta/index/admin/+param</t>
+  </si>
+  <si>
+    <t>Vista formulario de alta de nueva Encuesta, al terminar redirecciona a encuesta/index/</t>
+  </si>
+  <si>
+    <t>Muestra las secciones que contiene la encuesta, navegación a encuesta/seccion/alta/+param y encuesta/seccion/admin/+param</t>
+  </si>
+  <si>
+    <t>Mostrar detalle de encuesta, navegación a encuesta/index/edita y encuesta/secciones/+param</t>
+  </si>
+  <si>
+    <t>Mostrar detalle de seccion, navegación a encuesta/seccion/edita/+param, encuesta/seccion/baja/+param, encuesta/seccion/index/+param</t>
+  </si>
+  <si>
+    <t>Muestra grupos y preguntas de la seccion, navegación a encuesta/seccion/alta/+param, encuesta/grupo/admin/+param, encuesta/pregunta/admin/+param</t>
+  </si>
+  <si>
+    <t>Alta de Seccion a Encuesta, redirecciona a encuesta/secciones/+param</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,10 +217,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,7 +317,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -245,7 +351,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -421,274 +526,735 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>7</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="F13:Q13"/>
+    <mergeCell ref="F14:Q14"/>
+    <mergeCell ref="F15:Q15"/>
+    <mergeCell ref="F7:Q7"/>
+    <mergeCell ref="F8:Q8"/>
+    <mergeCell ref="F9:Q9"/>
+    <mergeCell ref="F10:Q10"/>
+    <mergeCell ref="F11:Q11"/>
+    <mergeCell ref="F12:Q12"/>
+    <mergeCell ref="F2:Q2"/>
+    <mergeCell ref="F3:Q3"/>
+    <mergeCell ref="F4:Q4"/>
+    <mergeCell ref="F5:Q5"/>
+    <mergeCell ref="F6:Q6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:B24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" s="5"/>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GiovanniPC: Lunes 22 de Febrero de 2016 x2
</commit_message>
<xml_diff>
--- a/docs/ControlPersistencia.xlsx
+++ b/docs/ControlPersistencia.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="14055" windowHeight="5130"/>
+    <workbookView xWindow="600" yWindow="90" windowWidth="14055" windowHeight="5130" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Persistencia" sheetId="3" r:id="rId3"/>
+    <sheet name="Sistema" sheetId="3" r:id="rId2"/>
+    <sheet name="Encuesta" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="54">
   <si>
     <t>Nombre</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>Alta de Seccion a Encuesta, redirecciona a encuesta/secciones/+param</t>
+  </si>
+  <si>
+    <t>Entidad</t>
+  </si>
+  <si>
+    <t>Nivel</t>
+  </si>
+  <si>
+    <t>Form</t>
   </si>
 </sst>
 </file>
@@ -220,14 +229,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14:Q14"/>
     </sheetView>
   </sheetViews>
@@ -575,20 +584,20 @@
       <c r="E2" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
@@ -606,20 +615,20 @@
       <c r="E3" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
@@ -637,20 +646,20 @@
       <c r="E4" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
@@ -662,26 +671,26 @@
       <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E5" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
@@ -693,26 +702,26 @@
       <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E6" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
@@ -730,20 +739,20 @@
       <c r="E7" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
@@ -761,20 +770,20 @@
       <c r="E8" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
@@ -792,20 +801,20 @@
       <c r="E9" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
@@ -823,93 +832,98 @@
       <c r="E10" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F2:Q2"/>
+    <mergeCell ref="F3:Q3"/>
+    <mergeCell ref="F4:Q4"/>
+    <mergeCell ref="F5:Q5"/>
+    <mergeCell ref="F6:Q6"/>
     <mergeCell ref="F13:Q13"/>
     <mergeCell ref="F14:Q14"/>
     <mergeCell ref="F15:Q15"/>
@@ -919,11 +933,6 @@
     <mergeCell ref="F10:Q10"/>
     <mergeCell ref="F11:Q11"/>
     <mergeCell ref="F12:Q12"/>
-    <mergeCell ref="F2:Q2"/>
-    <mergeCell ref="F3:Q3"/>
-    <mergeCell ref="F4:Q4"/>
-    <mergeCell ref="F5:Q5"/>
-    <mergeCell ref="F6:Q6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -932,82 +941,243 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:B24"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:2">
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3" spans="2:2">
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="2:2">
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="2:2">
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="2:2">
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="2:2">
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="2:2">
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="2:2">
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="2:2">
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="2:2">
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="2:2">
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="2:2">
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="2:2">
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="5"/>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1016,32 +1186,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
@@ -1049,10 +1219,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+        <v>52</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1063,196 +1233,72 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
-      </c>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" t="s">
-        <v>7</v>
-      </c>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>7</v>
-      </c>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s">
-        <v>7</v>
-      </c>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>7</v>
-      </c>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>